<commit_message>
routes added only 3 routes
</commit_message>
<xml_diff>
--- a/prices_updated.xlsx
+++ b/prices_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LocalAdmin\Desktop\Nabeel Ahmed Data Analyst\git\logenix_quote_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9993BBA0-A8D2-40E1-B779-0CFE6CEF70C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DDEB87-E23B-4C46-9C64-370B0BF3B2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4961" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5018" uniqueCount="658">
   <si>
     <t>S.No</t>
   </si>
@@ -1996,6 +1996,9 @@
   </si>
   <si>
     <t>Ocean Freight (40ft)</t>
+  </si>
+  <si>
+    <t>Almaty</t>
   </si>
 </sst>
 </file>
@@ -2034,7 +2037,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2183,6 +2186,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFACB9CA"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2671,7 +2686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="304">
+  <cellXfs count="311">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3201,6 +3216,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="26" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3221,58 +3251,58 @@
     <xf numFmtId="0" fontId="2" fillId="15" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="15" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="15" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="15" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="15" fontId="2" fillId="15" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="15" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="15" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="15" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3309,6 +3339,51 @@
     <xf numFmtId="15" fontId="2" fillId="23" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3318,51 +3393,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3486,8 +3516,6 @@
     <xf numFmtId="15" fontId="2" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3510,6 +3538,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3840,8 +3870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="G356" workbookViewId="0">
+      <selection activeCell="Q370" sqref="Q370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3855,6 +3885,7 @@
     <col min="7" max="7" width="58.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="16" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
@@ -5223,24 +5254,24 @@
       <c r="S24" s="3"/>
       <c r="T24" s="4"/>
     </row>
-    <row r="25" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="302">
+    <row r="25" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="309">
         <v>24</v>
       </c>
-      <c r="B25" s="300">
+      <c r="B25" s="307">
         <v>45971</v>
       </c>
-      <c r="C25" s="298"/>
-      <c r="D25" s="298" t="s">
+      <c r="C25" s="305"/>
+      <c r="D25" s="305" t="s">
         <v>85</v>
       </c>
-      <c r="E25" s="298" t="s">
+      <c r="E25" s="305" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="298" t="s">
+      <c r="F25" s="305" t="s">
         <v>87</v>
       </c>
-      <c r="G25" s="298" t="s">
+      <c r="G25" s="305" t="s">
         <v>88</v>
       </c>
       <c r="H25" s="19" t="s">
@@ -5249,61 +5280,61 @@
       <c r="I25" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="J25" s="298" t="s">
-        <v>19</v>
-      </c>
-      <c r="K25" s="298" t="s">
-        <v>19</v>
-      </c>
-      <c r="L25" s="298" t="s">
-        <v>19</v>
-      </c>
-      <c r="M25" s="298" t="s">
+      <c r="J25" s="305" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="305" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25" s="305" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" s="305" t="s">
         <v>22</v>
       </c>
-      <c r="N25" s="298" t="s">
-        <v>19</v>
-      </c>
-      <c r="O25" s="298" t="s">
-        <v>19</v>
-      </c>
-      <c r="P25" s="298" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q25" s="300">
+      <c r="N25" s="305" t="s">
+        <v>19</v>
+      </c>
+      <c r="O25" s="305" t="s">
+        <v>19</v>
+      </c>
+      <c r="P25" s="305" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q25" s="307">
         <v>45991</v>
       </c>
-      <c r="R25" s="298" t="s">
+      <c r="R25" s="305" t="s">
         <v>93</v>
       </c>
-      <c r="S25" s="286"/>
-      <c r="T25" s="286"/>
-    </row>
-    <row r="26" spans="1:20" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="303"/>
-      <c r="B26" s="301"/>
-      <c r="C26" s="299"/>
-      <c r="D26" s="299"/>
-      <c r="E26" s="299"/>
-      <c r="F26" s="299"/>
-      <c r="G26" s="299"/>
+      <c r="S25" s="291"/>
+      <c r="T25" s="291"/>
+    </row>
+    <row r="26" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="310"/>
+      <c r="B26" s="308"/>
+      <c r="C26" s="306"/>
+      <c r="D26" s="306"/>
+      <c r="E26" s="306"/>
+      <c r="F26" s="306"/>
+      <c r="G26" s="306"/>
       <c r="H26" s="20" t="s">
         <v>90</v>
       </c>
       <c r="I26" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="J26" s="299"/>
-      <c r="K26" s="299"/>
-      <c r="L26" s="299"/>
-      <c r="M26" s="299"/>
-      <c r="N26" s="299"/>
-      <c r="O26" s="299"/>
-      <c r="P26" s="299"/>
-      <c r="Q26" s="301"/>
-      <c r="R26" s="299"/>
-      <c r="S26" s="287"/>
-      <c r="T26" s="287"/>
+      <c r="J26" s="306"/>
+      <c r="K26" s="306"/>
+      <c r="L26" s="306"/>
+      <c r="M26" s="306"/>
+      <c r="N26" s="306"/>
+      <c r="O26" s="306"/>
+      <c r="P26" s="306"/>
+      <c r="Q26" s="308"/>
+      <c r="R26" s="306"/>
+      <c r="S26" s="292"/>
+      <c r="T26" s="292"/>
     </row>
     <row r="27" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="21">
@@ -5474,23 +5505,23 @@
       <c r="T29" s="4"/>
     </row>
     <row r="30" spans="1:20" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="302">
+      <c r="A30" s="309">
         <v>28</v>
       </c>
-      <c r="B30" s="300">
+      <c r="B30" s="307">
         <v>45971</v>
       </c>
-      <c r="C30" s="298"/>
-      <c r="D30" s="298" t="s">
+      <c r="C30" s="305"/>
+      <c r="D30" s="305" t="s">
         <v>85</v>
       </c>
-      <c r="E30" s="298" t="s">
+      <c r="E30" s="305" t="s">
         <v>97</v>
       </c>
-      <c r="F30" s="298" t="s">
+      <c r="F30" s="305" t="s">
         <v>87</v>
       </c>
-      <c r="G30" s="298" t="s">
+      <c r="G30" s="305" t="s">
         <v>88</v>
       </c>
       <c r="H30" s="19" t="s">
@@ -5499,84 +5530,84 @@
       <c r="I30" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="J30" s="298" t="s">
-        <v>19</v>
-      </c>
-      <c r="K30" s="298" t="s">
-        <v>19</v>
-      </c>
-      <c r="L30" s="298" t="s">
-        <v>19</v>
-      </c>
-      <c r="M30" s="298" t="s">
+      <c r="J30" s="305" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" s="305" t="s">
+        <v>19</v>
+      </c>
+      <c r="L30" s="305" t="s">
+        <v>19</v>
+      </c>
+      <c r="M30" s="305" t="s">
         <v>22</v>
       </c>
       <c r="N30" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="O30" s="298" t="s">
+      <c r="O30" s="305" t="s">
         <v>19</v>
       </c>
       <c r="P30" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="Q30" s="300">
+      <c r="Q30" s="307">
         <v>45991</v>
       </c>
-      <c r="R30" s="298" t="s">
+      <c r="R30" s="305" t="s">
         <v>93</v>
       </c>
-      <c r="S30" s="286"/>
-      <c r="T30" s="286"/>
+      <c r="S30" s="291"/>
+      <c r="T30" s="291"/>
     </row>
     <row r="31" spans="1:20" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="303"/>
-      <c r="B31" s="301"/>
-      <c r="C31" s="299"/>
-      <c r="D31" s="299"/>
-      <c r="E31" s="299"/>
-      <c r="F31" s="299"/>
-      <c r="G31" s="299"/>
+      <c r="A31" s="310"/>
+      <c r="B31" s="308"/>
+      <c r="C31" s="306"/>
+      <c r="D31" s="306"/>
+      <c r="E31" s="306"/>
+      <c r="F31" s="306"/>
+      <c r="G31" s="306"/>
       <c r="H31" s="20" t="s">
         <v>99</v>
       </c>
       <c r="I31" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="J31" s="299"/>
-      <c r="K31" s="299"/>
-      <c r="L31" s="299"/>
-      <c r="M31" s="299"/>
+      <c r="J31" s="306"/>
+      <c r="K31" s="306"/>
+      <c r="L31" s="306"/>
+      <c r="M31" s="306"/>
       <c r="N31" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="O31" s="299"/>
+      <c r="O31" s="306"/>
       <c r="P31" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="Q31" s="301"/>
-      <c r="R31" s="299"/>
-      <c r="S31" s="287"/>
-      <c r="T31" s="287"/>
+      <c r="Q31" s="308"/>
+      <c r="R31" s="306"/>
+      <c r="S31" s="292"/>
+      <c r="T31" s="292"/>
     </row>
     <row r="32" spans="1:20" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="302">
+      <c r="A32" s="309">
         <v>29</v>
       </c>
-      <c r="B32" s="300">
+      <c r="B32" s="307">
         <v>45971</v>
       </c>
-      <c r="C32" s="298"/>
-      <c r="D32" s="298" t="s">
+      <c r="C32" s="305"/>
+      <c r="D32" s="305" t="s">
         <v>85</v>
       </c>
-      <c r="E32" s="298" t="s">
+      <c r="E32" s="305" t="s">
         <v>97</v>
       </c>
-      <c r="F32" s="298" t="s">
+      <c r="F32" s="305" t="s">
         <v>87</v>
       </c>
-      <c r="G32" s="298" t="s">
+      <c r="G32" s="305" t="s">
         <v>88</v>
       </c>
       <c r="H32" s="19" t="s">
@@ -5585,65 +5616,65 @@
       <c r="I32" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="J32" s="298" t="s">
-        <v>19</v>
-      </c>
-      <c r="K32" s="298" t="s">
-        <v>19</v>
-      </c>
-      <c r="L32" s="298" t="s">
-        <v>19</v>
-      </c>
-      <c r="M32" s="298" t="s">
+      <c r="J32" s="305" t="s">
+        <v>19</v>
+      </c>
+      <c r="K32" s="305" t="s">
+        <v>19</v>
+      </c>
+      <c r="L32" s="305" t="s">
+        <v>19</v>
+      </c>
+      <c r="M32" s="305" t="s">
         <v>22</v>
       </c>
-      <c r="N32" s="298" t="s">
+      <c r="N32" s="305" t="s">
         <v>56</v>
       </c>
-      <c r="O32" s="298" t="s">
+      <c r="O32" s="305" t="s">
         <v>19</v>
       </c>
       <c r="P32" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="Q32" s="300">
+      <c r="Q32" s="307">
         <v>45991</v>
       </c>
-      <c r="R32" s="298" t="s">
+      <c r="R32" s="305" t="s">
         <v>93</v>
       </c>
-      <c r="S32" s="286"/>
-      <c r="T32" s="286"/>
+      <c r="S32" s="291"/>
+      <c r="T32" s="291"/>
     </row>
     <row r="33" spans="1:20" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="303"/>
-      <c r="B33" s="301"/>
-      <c r="C33" s="299"/>
-      <c r="D33" s="299"/>
-      <c r="E33" s="299"/>
-      <c r="F33" s="299"/>
-      <c r="G33" s="299"/>
+      <c r="A33" s="310"/>
+      <c r="B33" s="308"/>
+      <c r="C33" s="306"/>
+      <c r="D33" s="306"/>
+      <c r="E33" s="306"/>
+      <c r="F33" s="306"/>
+      <c r="G33" s="306"/>
       <c r="H33" s="20" t="s">
         <v>107</v>
       </c>
       <c r="I33" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="J33" s="299"/>
-      <c r="K33" s="299"/>
-      <c r="L33" s="299"/>
-      <c r="M33" s="299"/>
-      <c r="N33" s="299"/>
-      <c r="O33" s="299"/>
+      <c r="J33" s="306"/>
+      <c r="K33" s="306"/>
+      <c r="L33" s="306"/>
+      <c r="M33" s="306"/>
+      <c r="N33" s="306"/>
+      <c r="O33" s="306"/>
       <c r="P33" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="Q33" s="301"/>
-      <c r="R33" s="299"/>
-      <c r="S33" s="287"/>
-      <c r="T33" s="287"/>
-    </row>
-    <row r="34" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="Q33" s="308"/>
+      <c r="R33" s="306"/>
+      <c r="S33" s="292"/>
+      <c r="T33" s="292"/>
+    </row>
+    <row r="34" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="21">
         <v>30</v>
       </c>
@@ -5879,10 +5910,10 @@
       <c r="G38" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="H38" s="294" t="s">
+      <c r="H38" s="301" t="s">
         <v>122</v>
       </c>
-      <c r="I38" s="295"/>
+      <c r="I38" s="302"/>
       <c r="J38" s="27" t="s">
         <v>19</v>
       </c>
@@ -5933,10 +5964,10 @@
       <c r="G39" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="H39" s="294" t="s">
+      <c r="H39" s="301" t="s">
         <v>124</v>
       </c>
-      <c r="I39" s="295"/>
+      <c r="I39" s="302"/>
       <c r="J39" s="27" t="s">
         <v>19</v>
       </c>
@@ -5987,10 +6018,10 @@
       <c r="G40" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="H40" s="294" t="s">
+      <c r="H40" s="301" t="s">
         <v>126</v>
       </c>
-      <c r="I40" s="295"/>
+      <c r="I40" s="302"/>
       <c r="J40" s="27" t="s">
         <v>19</v>
       </c>
@@ -6041,10 +6072,10 @@
       <c r="G41" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="H41" s="294" t="s">
+      <c r="H41" s="301" t="s">
         <v>128</v>
       </c>
-      <c r="I41" s="295"/>
+      <c r="I41" s="302"/>
       <c r="J41" s="27" t="s">
         <v>19</v>
       </c>
@@ -6095,10 +6126,10 @@
       <c r="G42" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="H42" s="294" t="s">
+      <c r="H42" s="301" t="s">
         <v>130</v>
       </c>
-      <c r="I42" s="295"/>
+      <c r="I42" s="302"/>
       <c r="J42" s="27" t="s">
         <v>19</v>
       </c>
@@ -6481,10 +6512,10 @@
       <c r="G49" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="H49" s="296" t="s">
+      <c r="H49" s="303" t="s">
         <v>140</v>
       </c>
-      <c r="I49" s="296" t="s">
+      <c r="I49" s="303" t="s">
         <v>141</v>
       </c>
       <c r="J49" s="33" t="s">
@@ -6537,8 +6568,8 @@
       <c r="G50" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="H50" s="297"/>
-      <c r="I50" s="297"/>
+      <c r="H50" s="304"/>
+      <c r="I50" s="304"/>
       <c r="J50" s="33" t="s">
         <v>144</v>
       </c>
@@ -7093,12 +7124,12 @@
       <c r="G60" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="H60" s="288" t="s">
-        <v>19</v>
-      </c>
-      <c r="I60" s="289"/>
-      <c r="J60" s="289"/>
-      <c r="K60" s="290"/>
+      <c r="H60" s="295" t="s">
+        <v>19</v>
+      </c>
+      <c r="I60" s="296"/>
+      <c r="J60" s="296"/>
+      <c r="K60" s="297"/>
       <c r="L60" s="23" t="s">
         <v>19</v>
       </c>
@@ -7143,12 +7174,12 @@
       <c r="G61" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="H61" s="288" t="s">
-        <v>19</v>
-      </c>
-      <c r="I61" s="289"/>
-      <c r="J61" s="289"/>
-      <c r="K61" s="290"/>
+      <c r="H61" s="295" t="s">
+        <v>19</v>
+      </c>
+      <c r="I61" s="296"/>
+      <c r="J61" s="296"/>
+      <c r="K61" s="297"/>
       <c r="L61" s="23" t="s">
         <v>19</v>
       </c>
@@ -7193,12 +7224,12 @@
       <c r="G62" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="H62" s="288" t="s">
-        <v>19</v>
-      </c>
-      <c r="I62" s="289"/>
-      <c r="J62" s="289"/>
-      <c r="K62" s="290"/>
+      <c r="H62" s="295" t="s">
+        <v>19</v>
+      </c>
+      <c r="I62" s="296"/>
+      <c r="J62" s="296"/>
+      <c r="K62" s="297"/>
       <c r="L62" s="23" t="s">
         <v>19</v>
       </c>
@@ -7243,12 +7274,12 @@
       <c r="G63" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="H63" s="291" t="s">
+      <c r="H63" s="298" t="s">
         <v>164</v>
       </c>
-      <c r="I63" s="292"/>
-      <c r="J63" s="292"/>
-      <c r="K63" s="293"/>
+      <c r="I63" s="299"/>
+      <c r="J63" s="299"/>
+      <c r="K63" s="300"/>
       <c r="L63" s="23" t="s">
         <v>19</v>
       </c>
@@ -7778,422 +7809,422 @@
       <c r="T72" s="4"/>
     </row>
     <row r="73" spans="1:20" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="272">
+      <c r="A73" s="279">
         <v>69</v>
       </c>
-      <c r="B73" s="274">
+      <c r="B73" s="281">
         <v>45972</v>
       </c>
-      <c r="C73" s="264"/>
-      <c r="D73" s="264" t="s">
+      <c r="C73" s="271"/>
+      <c r="D73" s="271" t="s">
         <v>165</v>
       </c>
-      <c r="E73" s="264" t="s">
+      <c r="E73" s="271" t="s">
         <v>179</v>
       </c>
-      <c r="F73" s="264" t="s">
+      <c r="F73" s="271" t="s">
         <v>18</v>
       </c>
-      <c r="G73" s="264" t="s">
+      <c r="G73" s="271" t="s">
         <v>185</v>
       </c>
-      <c r="H73" s="266" t="s">
+      <c r="H73" s="273" t="s">
         <v>186</v>
       </c>
-      <c r="I73" s="267"/>
-      <c r="J73" s="267"/>
-      <c r="K73" s="268"/>
-      <c r="L73" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="M73" s="264" t="s">
+      <c r="I73" s="274"/>
+      <c r="J73" s="274"/>
+      <c r="K73" s="275"/>
+      <c r="L73" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="M73" s="271" t="s">
         <v>22</v>
       </c>
-      <c r="N73" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="O73" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="P73" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q73" s="274">
+      <c r="N73" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="O73" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="P73" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q73" s="281">
         <v>45983</v>
       </c>
-      <c r="R73" s="264" t="s">
+      <c r="R73" s="271" t="s">
         <v>169</v>
       </c>
-      <c r="S73" s="286"/>
-      <c r="T73" s="286"/>
+      <c r="S73" s="291"/>
+      <c r="T73" s="291"/>
     </row>
     <row r="74" spans="1:20" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="273"/>
-      <c r="B74" s="275"/>
-      <c r="C74" s="265"/>
-      <c r="D74" s="265"/>
-      <c r="E74" s="265"/>
-      <c r="F74" s="265"/>
-      <c r="G74" s="265"/>
-      <c r="H74" s="269" t="s">
+      <c r="A74" s="280"/>
+      <c r="B74" s="282"/>
+      <c r="C74" s="272"/>
+      <c r="D74" s="272"/>
+      <c r="E74" s="272"/>
+      <c r="F74" s="272"/>
+      <c r="G74" s="272"/>
+      <c r="H74" s="276" t="s">
         <v>187</v>
       </c>
-      <c r="I74" s="270"/>
-      <c r="J74" s="270"/>
-      <c r="K74" s="271"/>
-      <c r="L74" s="265"/>
-      <c r="M74" s="265"/>
-      <c r="N74" s="265"/>
-      <c r="O74" s="265"/>
-      <c r="P74" s="265"/>
-      <c r="Q74" s="275"/>
-      <c r="R74" s="265"/>
-      <c r="S74" s="287"/>
-      <c r="T74" s="287"/>
+      <c r="I74" s="277"/>
+      <c r="J74" s="277"/>
+      <c r="K74" s="278"/>
+      <c r="L74" s="272"/>
+      <c r="M74" s="272"/>
+      <c r="N74" s="272"/>
+      <c r="O74" s="272"/>
+      <c r="P74" s="272"/>
+      <c r="Q74" s="282"/>
+      <c r="R74" s="272"/>
+      <c r="S74" s="292"/>
+      <c r="T74" s="292"/>
     </row>
     <row r="75" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="272">
+      <c r="A75" s="279">
         <v>70</v>
       </c>
-      <c r="B75" s="274">
+      <c r="B75" s="281">
         <v>45972</v>
       </c>
-      <c r="C75" s="264"/>
-      <c r="D75" s="264" t="s">
+      <c r="C75" s="271"/>
+      <c r="D75" s="271" t="s">
         <v>165</v>
       </c>
-      <c r="E75" s="264" t="s">
+      <c r="E75" s="271" t="s">
         <v>179</v>
       </c>
-      <c r="F75" s="264" t="s">
+      <c r="F75" s="271" t="s">
         <v>18</v>
       </c>
-      <c r="G75" s="264" t="s">
+      <c r="G75" s="271" t="s">
         <v>188</v>
       </c>
-      <c r="H75" s="266" t="s">
+      <c r="H75" s="273" t="s">
         <v>189</v>
       </c>
-      <c r="I75" s="267"/>
-      <c r="J75" s="267"/>
-      <c r="K75" s="268"/>
-      <c r="L75" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="M75" s="264" t="s">
+      <c r="I75" s="274"/>
+      <c r="J75" s="274"/>
+      <c r="K75" s="275"/>
+      <c r="L75" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="M75" s="271" t="s">
         <v>22</v>
       </c>
-      <c r="N75" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="O75" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="P75" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q75" s="274">
+      <c r="N75" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="O75" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="P75" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q75" s="281">
         <v>45983</v>
       </c>
-      <c r="R75" s="264" t="s">
+      <c r="R75" s="271" t="s">
         <v>169</v>
       </c>
-      <c r="S75" s="276"/>
-      <c r="T75" s="278"/>
+      <c r="S75" s="293"/>
+      <c r="T75" s="283"/>
     </row>
     <row r="76" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="285"/>
-      <c r="B76" s="281"/>
-      <c r="C76" s="280"/>
-      <c r="D76" s="280"/>
-      <c r="E76" s="280"/>
-      <c r="F76" s="280"/>
-      <c r="G76" s="280"/>
-      <c r="H76" s="282" t="s">
+      <c r="A76" s="290"/>
+      <c r="B76" s="286"/>
+      <c r="C76" s="285"/>
+      <c r="D76" s="285"/>
+      <c r="E76" s="285"/>
+      <c r="F76" s="285"/>
+      <c r="G76" s="285"/>
+      <c r="H76" s="287" t="s">
         <v>190</v>
       </c>
-      <c r="I76" s="283"/>
-      <c r="J76" s="283"/>
-      <c r="K76" s="284"/>
-      <c r="L76" s="280"/>
-      <c r="M76" s="280"/>
-      <c r="N76" s="280"/>
-      <c r="O76" s="280"/>
-      <c r="P76" s="280"/>
-      <c r="Q76" s="281"/>
-      <c r="R76" s="280"/>
-      <c r="S76" s="277"/>
-      <c r="T76" s="279"/>
+      <c r="I76" s="288"/>
+      <c r="J76" s="288"/>
+      <c r="K76" s="289"/>
+      <c r="L76" s="285"/>
+      <c r="M76" s="285"/>
+      <c r="N76" s="285"/>
+      <c r="O76" s="285"/>
+      <c r="P76" s="285"/>
+      <c r="Q76" s="286"/>
+      <c r="R76" s="285"/>
+      <c r="S76" s="294"/>
+      <c r="T76" s="284"/>
     </row>
     <row r="77" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="285"/>
-      <c r="B77" s="281"/>
-      <c r="C77" s="280"/>
-      <c r="D77" s="280"/>
-      <c r="E77" s="280"/>
-      <c r="F77" s="280"/>
-      <c r="G77" s="280"/>
-      <c r="H77" s="282" t="s">
+      <c r="A77" s="290"/>
+      <c r="B77" s="286"/>
+      <c r="C77" s="285"/>
+      <c r="D77" s="285"/>
+      <c r="E77" s="285"/>
+      <c r="F77" s="285"/>
+      <c r="G77" s="285"/>
+      <c r="H77" s="287" t="s">
         <v>191</v>
       </c>
-      <c r="I77" s="283"/>
-      <c r="J77" s="283"/>
-      <c r="K77" s="284"/>
-      <c r="L77" s="280"/>
-      <c r="M77" s="280"/>
-      <c r="N77" s="280"/>
-      <c r="O77" s="280"/>
-      <c r="P77" s="280"/>
-      <c r="Q77" s="281"/>
-      <c r="R77" s="280"/>
-      <c r="S77" s="277"/>
-      <c r="T77" s="279"/>
+      <c r="I77" s="288"/>
+      <c r="J77" s="288"/>
+      <c r="K77" s="289"/>
+      <c r="L77" s="285"/>
+      <c r="M77" s="285"/>
+      <c r="N77" s="285"/>
+      <c r="O77" s="285"/>
+      <c r="P77" s="285"/>
+      <c r="Q77" s="286"/>
+      <c r="R77" s="285"/>
+      <c r="S77" s="294"/>
+      <c r="T77" s="284"/>
     </row>
     <row r="78" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="273"/>
-      <c r="B78" s="275"/>
-      <c r="C78" s="265"/>
-      <c r="D78" s="265"/>
-      <c r="E78" s="265"/>
-      <c r="F78" s="265"/>
-      <c r="G78" s="265"/>
-      <c r="H78" s="269" t="s">
+      <c r="A78" s="280"/>
+      <c r="B78" s="282"/>
+      <c r="C78" s="272"/>
+      <c r="D78" s="272"/>
+      <c r="E78" s="272"/>
+      <c r="F78" s="272"/>
+      <c r="G78" s="272"/>
+      <c r="H78" s="276" t="s">
         <v>192</v>
       </c>
-      <c r="I78" s="270"/>
-      <c r="J78" s="270"/>
-      <c r="K78" s="271"/>
-      <c r="L78" s="265"/>
-      <c r="M78" s="265"/>
-      <c r="N78" s="265"/>
-      <c r="O78" s="265"/>
-      <c r="P78" s="265"/>
-      <c r="Q78" s="275"/>
-      <c r="R78" s="265"/>
-      <c r="S78" s="277"/>
-      <c r="T78" s="279"/>
+      <c r="I78" s="277"/>
+      <c r="J78" s="277"/>
+      <c r="K78" s="278"/>
+      <c r="L78" s="272"/>
+      <c r="M78" s="272"/>
+      <c r="N78" s="272"/>
+      <c r="O78" s="272"/>
+      <c r="P78" s="272"/>
+      <c r="Q78" s="282"/>
+      <c r="R78" s="272"/>
+      <c r="S78" s="294"/>
+      <c r="T78" s="284"/>
     </row>
     <row r="79" spans="1:20" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="272">
+      <c r="A79" s="279">
         <v>71</v>
       </c>
-      <c r="B79" s="274">
+      <c r="B79" s="281">
         <v>45972</v>
       </c>
-      <c r="C79" s="264"/>
-      <c r="D79" s="264" t="s">
+      <c r="C79" s="271"/>
+      <c r="D79" s="271" t="s">
         <v>165</v>
       </c>
-      <c r="E79" s="264" t="s">
+      <c r="E79" s="271" t="s">
         <v>193</v>
       </c>
-      <c r="F79" s="264" t="s">
+      <c r="F79" s="271" t="s">
         <v>18</v>
       </c>
-      <c r="G79" s="264" t="s">
+      <c r="G79" s="271" t="s">
         <v>185</v>
       </c>
-      <c r="H79" s="266" t="s">
+      <c r="H79" s="273" t="s">
         <v>194</v>
       </c>
-      <c r="I79" s="267"/>
-      <c r="J79" s="267"/>
-      <c r="K79" s="268"/>
-      <c r="L79" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="M79" s="264" t="s">
+      <c r="I79" s="274"/>
+      <c r="J79" s="274"/>
+      <c r="K79" s="275"/>
+      <c r="L79" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="M79" s="271" t="s">
         <v>22</v>
       </c>
-      <c r="N79" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="O79" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="P79" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q79" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="R79" s="264" t="s">
+      <c r="N79" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="O79" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="P79" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q79" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="R79" s="271" t="s">
         <v>169</v>
       </c>
-      <c r="S79" s="193"/>
-      <c r="T79" s="179"/>
+      <c r="S79" s="210"/>
+      <c r="T79" s="186"/>
     </row>
     <row r="80" spans="1:20" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="273"/>
-      <c r="B80" s="275"/>
-      <c r="C80" s="265"/>
-      <c r="D80" s="265"/>
-      <c r="E80" s="265"/>
-      <c r="F80" s="265"/>
-      <c r="G80" s="265"/>
-      <c r="H80" s="269" t="s">
+      <c r="A80" s="280"/>
+      <c r="B80" s="282"/>
+      <c r="C80" s="272"/>
+      <c r="D80" s="272"/>
+      <c r="E80" s="272"/>
+      <c r="F80" s="272"/>
+      <c r="G80" s="272"/>
+      <c r="H80" s="276" t="s">
         <v>195</v>
       </c>
-      <c r="I80" s="270"/>
-      <c r="J80" s="270"/>
-      <c r="K80" s="271"/>
-      <c r="L80" s="265"/>
-      <c r="M80" s="265"/>
-      <c r="N80" s="265"/>
-      <c r="O80" s="265"/>
-      <c r="P80" s="265"/>
-      <c r="Q80" s="265"/>
-      <c r="R80" s="265"/>
-      <c r="S80" s="193"/>
-      <c r="T80" s="179"/>
+      <c r="I80" s="277"/>
+      <c r="J80" s="277"/>
+      <c r="K80" s="278"/>
+      <c r="L80" s="272"/>
+      <c r="M80" s="272"/>
+      <c r="N80" s="272"/>
+      <c r="O80" s="272"/>
+      <c r="P80" s="272"/>
+      <c r="Q80" s="272"/>
+      <c r="R80" s="272"/>
+      <c r="S80" s="210"/>
+      <c r="T80" s="186"/>
     </row>
     <row r="81" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="272">
+      <c r="A81" s="279">
         <v>72</v>
       </c>
-      <c r="B81" s="274">
+      <c r="B81" s="281">
         <v>45972</v>
       </c>
-      <c r="C81" s="264"/>
-      <c r="D81" s="264" t="s">
+      <c r="C81" s="271"/>
+      <c r="D81" s="271" t="s">
         <v>165</v>
       </c>
-      <c r="E81" s="264" t="s">
+      <c r="E81" s="271" t="s">
         <v>196</v>
       </c>
-      <c r="F81" s="264" t="s">
+      <c r="F81" s="271" t="s">
         <v>18</v>
       </c>
-      <c r="G81" s="264" t="s">
+      <c r="G81" s="271" t="s">
         <v>185</v>
       </c>
-      <c r="H81" s="266" t="s">
+      <c r="H81" s="273" t="s">
         <v>197</v>
       </c>
-      <c r="I81" s="267"/>
-      <c r="J81" s="267"/>
-      <c r="K81" s="268"/>
-      <c r="L81" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="M81" s="264" t="s">
+      <c r="I81" s="274"/>
+      <c r="J81" s="274"/>
+      <c r="K81" s="275"/>
+      <c r="L81" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="M81" s="271" t="s">
         <v>22</v>
       </c>
-      <c r="N81" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="O81" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="P81" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q81" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="R81" s="264" t="s">
+      <c r="N81" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="O81" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="P81" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q81" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="R81" s="271" t="s">
         <v>169</v>
       </c>
-      <c r="S81" s="193"/>
-      <c r="T81" s="179"/>
+      <c r="S81" s="210"/>
+      <c r="T81" s="186"/>
     </row>
     <row r="82" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="273"/>
-      <c r="B82" s="275"/>
-      <c r="C82" s="265"/>
-      <c r="D82" s="265"/>
-      <c r="E82" s="265"/>
-      <c r="F82" s="265"/>
-      <c r="G82" s="265"/>
-      <c r="H82" s="269" t="s">
+      <c r="A82" s="280"/>
+      <c r="B82" s="282"/>
+      <c r="C82" s="272"/>
+      <c r="D82" s="272"/>
+      <c r="E82" s="272"/>
+      <c r="F82" s="272"/>
+      <c r="G82" s="272"/>
+      <c r="H82" s="276" t="s">
         <v>198</v>
       </c>
-      <c r="I82" s="270"/>
-      <c r="J82" s="270"/>
-      <c r="K82" s="271"/>
-      <c r="L82" s="265"/>
-      <c r="M82" s="265"/>
-      <c r="N82" s="265"/>
-      <c r="O82" s="265"/>
-      <c r="P82" s="265"/>
-      <c r="Q82" s="265"/>
-      <c r="R82" s="265"/>
-      <c r="S82" s="193"/>
-      <c r="T82" s="179"/>
+      <c r="I82" s="277"/>
+      <c r="J82" s="277"/>
+      <c r="K82" s="278"/>
+      <c r="L82" s="272"/>
+      <c r="M82" s="272"/>
+      <c r="N82" s="272"/>
+      <c r="O82" s="272"/>
+      <c r="P82" s="272"/>
+      <c r="Q82" s="272"/>
+      <c r="R82" s="272"/>
+      <c r="S82" s="210"/>
+      <c r="T82" s="186"/>
     </row>
     <row r="83" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="272">
+      <c r="A83" s="279">
         <v>73</v>
       </c>
-      <c r="B83" s="274">
+      <c r="B83" s="281">
         <v>45972</v>
       </c>
-      <c r="C83" s="264"/>
-      <c r="D83" s="264" t="s">
+      <c r="C83" s="271"/>
+      <c r="D83" s="271" t="s">
         <v>165</v>
       </c>
-      <c r="E83" s="264" t="s">
+      <c r="E83" s="271" t="s">
         <v>196</v>
       </c>
-      <c r="F83" s="264" t="s">
+      <c r="F83" s="271" t="s">
         <v>18</v>
       </c>
-      <c r="G83" s="264" t="s">
+      <c r="G83" s="271" t="s">
         <v>185</v>
       </c>
-      <c r="H83" s="266" t="s">
+      <c r="H83" s="273" t="s">
         <v>199</v>
       </c>
-      <c r="I83" s="267"/>
-      <c r="J83" s="267"/>
-      <c r="K83" s="268"/>
-      <c r="L83" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="M83" s="264" t="s">
+      <c r="I83" s="274"/>
+      <c r="J83" s="274"/>
+      <c r="K83" s="275"/>
+      <c r="L83" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="M83" s="271" t="s">
         <v>22</v>
       </c>
-      <c r="N83" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="O83" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="P83" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q83" s="264" t="s">
-        <v>19</v>
-      </c>
-      <c r="R83" s="264" t="s">
+      <c r="N83" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="O83" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="P83" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q83" s="271" t="s">
+        <v>19</v>
+      </c>
+      <c r="R83" s="271" t="s">
         <v>169</v>
       </c>
-      <c r="S83" s="193"/>
-      <c r="T83" s="179"/>
+      <c r="S83" s="210"/>
+      <c r="T83" s="186"/>
     </row>
     <row r="84" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="273"/>
-      <c r="B84" s="275"/>
-      <c r="C84" s="265"/>
-      <c r="D84" s="265"/>
-      <c r="E84" s="265"/>
-      <c r="F84" s="265"/>
-      <c r="G84" s="265"/>
-      <c r="H84" s="269" t="s">
+      <c r="A84" s="280"/>
+      <c r="B84" s="282"/>
+      <c r="C84" s="272"/>
+      <c r="D84" s="272"/>
+      <c r="E84" s="272"/>
+      <c r="F84" s="272"/>
+      <c r="G84" s="272"/>
+      <c r="H84" s="276" t="s">
         <v>200</v>
       </c>
-      <c r="I84" s="270"/>
-      <c r="J84" s="270"/>
-      <c r="K84" s="271"/>
-      <c r="L84" s="265"/>
-      <c r="M84" s="265"/>
-      <c r="N84" s="265"/>
-      <c r="O84" s="265"/>
-      <c r="P84" s="265"/>
-      <c r="Q84" s="265"/>
-      <c r="R84" s="265"/>
-      <c r="S84" s="193"/>
-      <c r="T84" s="179"/>
+      <c r="I84" s="277"/>
+      <c r="J84" s="277"/>
+      <c r="K84" s="278"/>
+      <c r="L84" s="272"/>
+      <c r="M84" s="272"/>
+      <c r="N84" s="272"/>
+      <c r="O84" s="272"/>
+      <c r="P84" s="272"/>
+      <c r="Q84" s="272"/>
+      <c r="R84" s="272"/>
+      <c r="S84" s="210"/>
+      <c r="T84" s="186"/>
     </row>
     <row r="85" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="51">
@@ -9808,29 +9839,29 @@
       <c r="T113" s="50"/>
     </row>
     <row r="114" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A114" s="262">
+      <c r="A114" s="269">
         <v>103</v>
       </c>
-      <c r="B114" s="256">
+      <c r="B114" s="263">
         <v>45974</v>
       </c>
-      <c r="C114" s="258"/>
-      <c r="D114" s="258" t="s">
+      <c r="C114" s="265"/>
+      <c r="D114" s="265" t="s">
         <v>246</v>
       </c>
-      <c r="E114" s="258" t="s">
+      <c r="E114" s="265" t="s">
         <v>251</v>
       </c>
-      <c r="F114" s="258" t="s">
+      <c r="F114" s="265" t="s">
         <v>248</v>
       </c>
-      <c r="G114" s="258" t="s">
+      <c r="G114" s="265" t="s">
         <v>249</v>
       </c>
-      <c r="H114" s="258" t="s">
-        <v>19</v>
-      </c>
-      <c r="I114" s="258" t="s">
+      <c r="H114" s="265" t="s">
+        <v>19</v>
+      </c>
+      <c r="I114" s="265" t="s">
         <v>19</v>
       </c>
       <c r="J114" s="67" t="s">
@@ -9839,59 +9870,59 @@
       <c r="K114" s="67" t="s">
         <v>254</v>
       </c>
-      <c r="L114" s="258" t="s">
-        <v>19</v>
-      </c>
-      <c r="M114" s="258" t="s">
+      <c r="L114" s="265" t="s">
+        <v>19</v>
+      </c>
+      <c r="M114" s="265" t="s">
         <v>22</v>
       </c>
       <c r="N114" s="67" t="s">
         <v>256</v>
       </c>
-      <c r="O114" s="258" t="s">
+      <c r="O114" s="265" t="s">
         <v>19</v>
       </c>
       <c r="P114" s="67" t="s">
         <v>258</v>
       </c>
-      <c r="Q114" s="256">
+      <c r="Q114" s="263">
         <v>45991</v>
       </c>
-      <c r="R114" s="258" t="s">
+      <c r="R114" s="265" t="s">
         <v>250</v>
       </c>
-      <c r="S114" s="193"/>
-      <c r="T114" s="179"/>
+      <c r="S114" s="210"/>
+      <c r="T114" s="186"/>
     </row>
     <row r="115" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A115" s="263"/>
-      <c r="B115" s="257"/>
-      <c r="C115" s="259"/>
-      <c r="D115" s="259"/>
-      <c r="E115" s="259"/>
-      <c r="F115" s="259"/>
-      <c r="G115" s="259"/>
-      <c r="H115" s="259"/>
-      <c r="I115" s="259"/>
+      <c r="A115" s="270"/>
+      <c r="B115" s="264"/>
+      <c r="C115" s="266"/>
+      <c r="D115" s="266"/>
+      <c r="E115" s="266"/>
+      <c r="F115" s="266"/>
+      <c r="G115" s="266"/>
+      <c r="H115" s="266"/>
+      <c r="I115" s="266"/>
       <c r="J115" s="68" t="s">
         <v>253</v>
       </c>
       <c r="K115" s="68" t="s">
         <v>255</v>
       </c>
-      <c r="L115" s="259"/>
-      <c r="M115" s="259"/>
+      <c r="L115" s="266"/>
+      <c r="M115" s="266"/>
       <c r="N115" s="68" t="s">
         <v>257</v>
       </c>
-      <c r="O115" s="259"/>
+      <c r="O115" s="266"/>
       <c r="P115" s="68" t="s">
         <v>259</v>
       </c>
-      <c r="Q115" s="257"/>
-      <c r="R115" s="259"/>
-      <c r="S115" s="193"/>
-      <c r="T115" s="179"/>
+      <c r="Q115" s="264"/>
+      <c r="R115" s="266"/>
+      <c r="S115" s="210"/>
+      <c r="T115" s="186"/>
     </row>
     <row r="116" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="63">
@@ -11238,29 +11269,29 @@
       <c r="T139" s="50"/>
     </row>
     <row r="140" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A140" s="260">
+      <c r="A140" s="267">
         <v>128</v>
       </c>
-      <c r="B140" s="254">
+      <c r="B140" s="261">
         <v>45974</v>
       </c>
-      <c r="C140" s="252"/>
-      <c r="D140" s="252" t="s">
+      <c r="C140" s="259"/>
+      <c r="D140" s="259" t="s">
         <v>292</v>
       </c>
-      <c r="E140" s="252" t="s">
+      <c r="E140" s="259" t="s">
         <v>139</v>
       </c>
-      <c r="F140" s="252" t="s">
+      <c r="F140" s="259" t="s">
         <v>293</v>
       </c>
-      <c r="G140" s="252" t="s">
+      <c r="G140" s="259" t="s">
         <v>17</v>
       </c>
-      <c r="H140" s="252" t="s">
+      <c r="H140" s="259" t="s">
         <v>295</v>
       </c>
-      <c r="I140" s="252" t="s">
+      <c r="I140" s="259" t="s">
         <v>296</v>
       </c>
       <c r="J140" s="77" t="s">
@@ -11269,55 +11300,55 @@
       <c r="K140" s="77" t="s">
         <v>302</v>
       </c>
-      <c r="L140" s="252" t="s">
-        <v>19</v>
-      </c>
-      <c r="M140" s="252" t="s">
+      <c r="L140" s="259" t="s">
+        <v>19</v>
+      </c>
+      <c r="M140" s="259" t="s">
         <v>22</v>
       </c>
-      <c r="N140" s="252" t="s">
+      <c r="N140" s="259" t="s">
         <v>56</v>
       </c>
-      <c r="O140" s="252" t="s">
+      <c r="O140" s="259" t="s">
         <v>29</v>
       </c>
-      <c r="P140" s="252" t="s">
+      <c r="P140" s="259" t="s">
         <v>299</v>
       </c>
-      <c r="Q140" s="254">
+      <c r="Q140" s="261">
         <v>45991</v>
       </c>
-      <c r="R140" s="252" t="s">
+      <c r="R140" s="259" t="s">
         <v>294</v>
       </c>
-      <c r="S140" s="193"/>
-      <c r="T140" s="179"/>
-    </row>
-    <row r="141" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A141" s="261"/>
-      <c r="B141" s="255"/>
-      <c r="C141" s="253"/>
-      <c r="D141" s="253"/>
-      <c r="E141" s="253"/>
-      <c r="F141" s="253"/>
-      <c r="G141" s="253"/>
-      <c r="H141" s="253"/>
-      <c r="I141" s="253"/>
+      <c r="S140" s="210"/>
+      <c r="T140" s="186"/>
+    </row>
+    <row r="141" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A141" s="268"/>
+      <c r="B141" s="262"/>
+      <c r="C141" s="260"/>
+      <c r="D141" s="260"/>
+      <c r="E141" s="260"/>
+      <c r="F141" s="260"/>
+      <c r="G141" s="260"/>
+      <c r="H141" s="260"/>
+      <c r="I141" s="260"/>
       <c r="J141" s="78" t="s">
         <v>301</v>
       </c>
       <c r="K141" s="78" t="s">
         <v>303</v>
       </c>
-      <c r="L141" s="253"/>
-      <c r="M141" s="253"/>
-      <c r="N141" s="253"/>
-      <c r="O141" s="253"/>
-      <c r="P141" s="253"/>
-      <c r="Q141" s="255"/>
-      <c r="R141" s="253"/>
-      <c r="S141" s="193"/>
-      <c r="T141" s="179"/>
+      <c r="L141" s="260"/>
+      <c r="M141" s="260"/>
+      <c r="N141" s="260"/>
+      <c r="O141" s="260"/>
+      <c r="P141" s="260"/>
+      <c r="Q141" s="262"/>
+      <c r="R141" s="260"/>
+      <c r="S141" s="210"/>
+      <c r="T141" s="186"/>
     </row>
     <row r="142" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="73">
@@ -14454,84 +14485,84 @@
       <c r="T197" s="50"/>
     </row>
     <row r="198" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A198" s="248">
+      <c r="A198" s="255">
         <v>185</v>
       </c>
-      <c r="B198" s="250">
+      <c r="B198" s="257">
         <v>45979</v>
       </c>
-      <c r="C198" s="244"/>
-      <c r="D198" s="244" t="s">
+      <c r="C198" s="251"/>
+      <c r="D198" s="251" t="s">
         <v>382</v>
       </c>
-      <c r="E198" s="244" t="s">
+      <c r="E198" s="251" t="s">
         <v>390</v>
       </c>
-      <c r="F198" s="244" t="s">
+      <c r="F198" s="251" t="s">
         <v>383</v>
       </c>
-      <c r="G198" s="244" t="s">
+      <c r="G198" s="251" t="s">
         <v>388</v>
       </c>
-      <c r="H198" s="244" t="s">
+      <c r="H198" s="251" t="s">
         <v>176</v>
       </c>
-      <c r="I198" s="244" t="s">
+      <c r="I198" s="251" t="s">
         <v>391</v>
       </c>
-      <c r="J198" s="244" t="s">
+      <c r="J198" s="251" t="s">
         <v>392</v>
       </c>
-      <c r="K198" s="244" t="s">
+      <c r="K198" s="251" t="s">
         <v>392</v>
       </c>
-      <c r="L198" s="244" t="s">
-        <v>19</v>
-      </c>
-      <c r="M198" s="244" t="s">
+      <c r="L198" s="251" t="s">
+        <v>19</v>
+      </c>
+      <c r="M198" s="251" t="s">
         <v>22</v>
       </c>
-      <c r="N198" s="244" t="s">
+      <c r="N198" s="251" t="s">
         <v>19</v>
       </c>
       <c r="O198" s="96" t="s">
         <v>393</v>
       </c>
-      <c r="P198" s="244" t="s">
+      <c r="P198" s="251" t="s">
         <v>308</v>
       </c>
-      <c r="Q198" s="246">
+      <c r="Q198" s="253">
         <v>45995</v>
       </c>
-      <c r="R198" s="244" t="s">
+      <c r="R198" s="251" t="s">
         <v>384</v>
       </c>
-      <c r="S198" s="193"/>
-      <c r="T198" s="179"/>
+      <c r="S198" s="210"/>
+      <c r="T198" s="186"/>
     </row>
     <row r="199" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A199" s="249"/>
-      <c r="B199" s="251"/>
-      <c r="C199" s="245"/>
-      <c r="D199" s="245"/>
-      <c r="E199" s="245"/>
-      <c r="F199" s="245"/>
-      <c r="G199" s="245"/>
-      <c r="H199" s="245"/>
-      <c r="I199" s="245"/>
-      <c r="J199" s="245"/>
-      <c r="K199" s="245"/>
-      <c r="L199" s="245"/>
-      <c r="M199" s="245"/>
-      <c r="N199" s="245"/>
+      <c r="A199" s="256"/>
+      <c r="B199" s="258"/>
+      <c r="C199" s="252"/>
+      <c r="D199" s="252"/>
+      <c r="E199" s="252"/>
+      <c r="F199" s="252"/>
+      <c r="G199" s="252"/>
+      <c r="H199" s="252"/>
+      <c r="I199" s="252"/>
+      <c r="J199" s="252"/>
+      <c r="K199" s="252"/>
+      <c r="L199" s="252"/>
+      <c r="M199" s="252"/>
+      <c r="N199" s="252"/>
       <c r="O199" s="97" t="s">
         <v>394</v>
       </c>
-      <c r="P199" s="245"/>
-      <c r="Q199" s="247"/>
-      <c r="R199" s="245"/>
-      <c r="S199" s="193"/>
-      <c r="T199" s="179"/>
+      <c r="P199" s="252"/>
+      <c r="Q199" s="254"/>
+      <c r="R199" s="252"/>
+      <c r="S199" s="210"/>
+      <c r="T199" s="186"/>
     </row>
     <row r="200" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A200" s="93">
@@ -15206,35 +15237,35 @@
       <c r="T211" s="50"/>
     </row>
     <row r="212" spans="1:20" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A212" s="229">
+      <c r="A212" s="233">
         <v>198</v>
       </c>
-      <c r="B212" s="232">
+      <c r="B212" s="236">
         <v>45979</v>
       </c>
-      <c r="C212" s="217"/>
-      <c r="D212" s="217" t="s">
+      <c r="C212" s="239"/>
+      <c r="D212" s="239" t="s">
         <v>407</v>
       </c>
-      <c r="E212" s="217" t="s">
+      <c r="E212" s="239" t="s">
         <v>412</v>
       </c>
-      <c r="F212" s="217" t="s">
+      <c r="F212" s="239" t="s">
         <v>409</v>
       </c>
-      <c r="G212" s="217" t="s">
+      <c r="G212" s="239" t="s">
         <v>410</v>
       </c>
-      <c r="H212" s="238" t="s">
+      <c r="H212" s="245" t="s">
         <v>413</v>
       </c>
-      <c r="I212" s="239"/>
-      <c r="J212" s="239"/>
-      <c r="K212" s="240"/>
-      <c r="L212" s="226" t="s">
-        <v>19</v>
-      </c>
-      <c r="M212" s="226" t="s">
+      <c r="I212" s="246"/>
+      <c r="J212" s="246"/>
+      <c r="K212" s="247"/>
+      <c r="L212" s="230" t="s">
+        <v>19</v>
+      </c>
+      <c r="M212" s="230" t="s">
         <v>22</v>
       </c>
       <c r="N212" s="98" t="s">
@@ -15246,31 +15277,31 @@
       <c r="P212" s="98" t="s">
         <v>422</v>
       </c>
-      <c r="Q212" s="226" t="s">
-        <v>19</v>
-      </c>
-      <c r="R212" s="217" t="s">
+      <c r="Q212" s="230" t="s">
+        <v>19</v>
+      </c>
+      <c r="R212" s="239" t="s">
         <v>411</v>
       </c>
-      <c r="S212" s="193"/>
-      <c r="T212" s="179"/>
+      <c r="S212" s="210"/>
+      <c r="T212" s="186"/>
     </row>
     <row r="213" spans="1:20" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A213" s="230"/>
-      <c r="B213" s="233"/>
-      <c r="C213" s="218"/>
-      <c r="D213" s="218"/>
-      <c r="E213" s="218"/>
-      <c r="F213" s="218"/>
-      <c r="G213" s="218"/>
-      <c r="H213" s="241" t="s">
+      <c r="A213" s="234"/>
+      <c r="B213" s="237"/>
+      <c r="C213" s="240"/>
+      <c r="D213" s="240"/>
+      <c r="E213" s="240"/>
+      <c r="F213" s="240"/>
+      <c r="G213" s="240"/>
+      <c r="H213" s="248" t="s">
         <v>414</v>
       </c>
-      <c r="I213" s="242"/>
-      <c r="J213" s="242"/>
-      <c r="K213" s="243"/>
-      <c r="L213" s="227"/>
-      <c r="M213" s="227"/>
+      <c r="I213" s="249"/>
+      <c r="J213" s="249"/>
+      <c r="K213" s="250"/>
+      <c r="L213" s="231"/>
+      <c r="M213" s="231"/>
       <c r="N213" s="99" t="s">
         <v>417</v>
       </c>
@@ -15280,27 +15311,27 @@
       <c r="P213" s="99" t="s">
         <v>423</v>
       </c>
-      <c r="Q213" s="227"/>
-      <c r="R213" s="218"/>
-      <c r="S213" s="193"/>
-      <c r="T213" s="179"/>
+      <c r="Q213" s="231"/>
+      <c r="R213" s="240"/>
+      <c r="S213" s="210"/>
+      <c r="T213" s="186"/>
     </row>
     <row r="214" spans="1:20" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A214" s="231"/>
-      <c r="B214" s="234"/>
-      <c r="C214" s="219"/>
-      <c r="D214" s="219"/>
-      <c r="E214" s="219"/>
-      <c r="F214" s="219"/>
-      <c r="G214" s="219"/>
-      <c r="H214" s="235" t="s">
+      <c r="A214" s="235"/>
+      <c r="B214" s="238"/>
+      <c r="C214" s="241"/>
+      <c r="D214" s="241"/>
+      <c r="E214" s="241"/>
+      <c r="F214" s="241"/>
+      <c r="G214" s="241"/>
+      <c r="H214" s="242" t="s">
         <v>415</v>
       </c>
-      <c r="I214" s="236"/>
-      <c r="J214" s="236"/>
-      <c r="K214" s="237"/>
-      <c r="L214" s="228"/>
-      <c r="M214" s="228"/>
+      <c r="I214" s="243"/>
+      <c r="J214" s="243"/>
+      <c r="K214" s="244"/>
+      <c r="L214" s="232"/>
+      <c r="M214" s="232"/>
       <c r="N214" s="100" t="s">
         <v>418</v>
       </c>
@@ -15310,35 +15341,35 @@
       <c r="P214" s="100" t="s">
         <v>424</v>
       </c>
-      <c r="Q214" s="228"/>
-      <c r="R214" s="219"/>
-      <c r="S214" s="193"/>
-      <c r="T214" s="179"/>
-    </row>
-    <row r="215" spans="1:20" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A215" s="229">
+      <c r="Q214" s="232"/>
+      <c r="R214" s="241"/>
+      <c r="S214" s="210"/>
+      <c r="T214" s="186"/>
+    </row>
+    <row r="215" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A215" s="233">
         <v>199</v>
       </c>
-      <c r="B215" s="232">
+      <c r="B215" s="236">
         <v>45979</v>
       </c>
-      <c r="C215" s="217"/>
-      <c r="D215" s="217" t="s">
+      <c r="C215" s="239"/>
+      <c r="D215" s="239" t="s">
         <v>407</v>
       </c>
-      <c r="E215" s="217" t="s">
+      <c r="E215" s="239" t="s">
         <v>425</v>
       </c>
-      <c r="F215" s="217" t="s">
+      <c r="F215" s="239" t="s">
         <v>409</v>
       </c>
-      <c r="G215" s="217" t="s">
+      <c r="G215" s="239" t="s">
         <v>410</v>
       </c>
-      <c r="H215" s="217" t="s">
-        <v>19</v>
-      </c>
-      <c r="I215" s="217" t="s">
+      <c r="H215" s="239" t="s">
+        <v>19</v>
+      </c>
+      <c r="I215" s="239" t="s">
         <v>19</v>
       </c>
       <c r="J215" s="98" t="s">
@@ -15347,81 +15378,81 @@
       <c r="K215" s="98" t="s">
         <v>429</v>
       </c>
-      <c r="L215" s="226" t="s">
-        <v>19</v>
-      </c>
-      <c r="M215" s="226" t="s">
+      <c r="L215" s="230" t="s">
+        <v>19</v>
+      </c>
+      <c r="M215" s="230" t="s">
         <v>22</v>
       </c>
-      <c r="N215" s="226" t="s">
-        <v>19</v>
-      </c>
-      <c r="O215" s="226" t="s">
-        <v>19</v>
-      </c>
-      <c r="P215" s="226" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q215" s="226" t="s">
-        <v>19</v>
-      </c>
-      <c r="R215" s="217" t="s">
+      <c r="N215" s="230" t="s">
+        <v>19</v>
+      </c>
+      <c r="O215" s="230" t="s">
+        <v>19</v>
+      </c>
+      <c r="P215" s="230" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q215" s="230" t="s">
+        <v>19</v>
+      </c>
+      <c r="R215" s="239" t="s">
         <v>411</v>
       </c>
-      <c r="S215" s="193"/>
-      <c r="T215" s="179"/>
-    </row>
-    <row r="216" spans="1:20" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A216" s="230"/>
-      <c r="B216" s="233"/>
-      <c r="C216" s="218"/>
-      <c r="D216" s="218"/>
-      <c r="E216" s="218"/>
-      <c r="F216" s="218"/>
-      <c r="G216" s="218"/>
-      <c r="H216" s="218"/>
-      <c r="I216" s="218"/>
+      <c r="S215" s="210"/>
+      <c r="T215" s="186"/>
+    </row>
+    <row r="216" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A216" s="234"/>
+      <c r="B216" s="237"/>
+      <c r="C216" s="240"/>
+      <c r="D216" s="240"/>
+      <c r="E216" s="240"/>
+      <c r="F216" s="240"/>
+      <c r="G216" s="240"/>
+      <c r="H216" s="240"/>
+      <c r="I216" s="240"/>
       <c r="J216" s="99" t="s">
         <v>427</v>
       </c>
       <c r="K216" s="99" t="s">
         <v>430</v>
       </c>
-      <c r="L216" s="227"/>
-      <c r="M216" s="227"/>
-      <c r="N216" s="227"/>
-      <c r="O216" s="227"/>
-      <c r="P216" s="227"/>
-      <c r="Q216" s="227"/>
-      <c r="R216" s="218"/>
-      <c r="S216" s="193"/>
-      <c r="T216" s="179"/>
-    </row>
-    <row r="217" spans="1:20" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A217" s="231"/>
-      <c r="B217" s="234"/>
-      <c r="C217" s="219"/>
-      <c r="D217" s="219"/>
-      <c r="E217" s="219"/>
-      <c r="F217" s="219"/>
-      <c r="G217" s="219"/>
-      <c r="H217" s="219"/>
-      <c r="I217" s="219"/>
+      <c r="L216" s="231"/>
+      <c r="M216" s="231"/>
+      <c r="N216" s="231"/>
+      <c r="O216" s="231"/>
+      <c r="P216" s="231"/>
+      <c r="Q216" s="231"/>
+      <c r="R216" s="240"/>
+      <c r="S216" s="210"/>
+      <c r="T216" s="186"/>
+    </row>
+    <row r="217" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A217" s="235"/>
+      <c r="B217" s="238"/>
+      <c r="C217" s="241"/>
+      <c r="D217" s="241"/>
+      <c r="E217" s="241"/>
+      <c r="F217" s="241"/>
+      <c r="G217" s="241"/>
+      <c r="H217" s="241"/>
+      <c r="I217" s="241"/>
       <c r="J217" s="100" t="s">
         <v>428</v>
       </c>
       <c r="K217" s="100" t="s">
         <v>431</v>
       </c>
-      <c r="L217" s="228"/>
-      <c r="M217" s="228"/>
-      <c r="N217" s="228"/>
-      <c r="O217" s="228"/>
-      <c r="P217" s="228"/>
-      <c r="Q217" s="228"/>
-      <c r="R217" s="219"/>
-      <c r="S217" s="193"/>
-      <c r="T217" s="179"/>
+      <c r="L217" s="232"/>
+      <c r="M217" s="232"/>
+      <c r="N217" s="232"/>
+      <c r="O217" s="232"/>
+      <c r="P217" s="232"/>
+      <c r="Q217" s="232"/>
+      <c r="R217" s="241"/>
+      <c r="S217" s="210"/>
+      <c r="T217" s="186"/>
     </row>
     <row r="218" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A218" s="28">
@@ -15555,12 +15586,12 @@
       <c r="G220" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="H220" s="220" t="s">
+      <c r="H220" s="224" t="s">
         <v>324</v>
       </c>
-      <c r="I220" s="221"/>
-      <c r="J220" s="221"/>
-      <c r="K220" s="222"/>
+      <c r="I220" s="225"/>
+      <c r="J220" s="225"/>
+      <c r="K220" s="226"/>
       <c r="L220" s="103" t="s">
         <v>19</v>
       </c>
@@ -15605,12 +15636,12 @@
       <c r="G221" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="H221" s="220" t="s">
+      <c r="H221" s="224" t="s">
         <v>438</v>
       </c>
-      <c r="I221" s="221"/>
-      <c r="J221" s="221"/>
-      <c r="K221" s="222"/>
+      <c r="I221" s="225"/>
+      <c r="J221" s="225"/>
+      <c r="K221" s="226"/>
       <c r="L221" s="103" t="s">
         <v>19</v>
       </c>
@@ -16101,12 +16132,12 @@
       <c r="G230" s="107" t="s">
         <v>453</v>
       </c>
-      <c r="H230" s="223" t="s">
+      <c r="H230" s="227" t="s">
         <v>454</v>
       </c>
-      <c r="I230" s="224"/>
-      <c r="J230" s="224"/>
-      <c r="K230" s="225"/>
+      <c r="I230" s="228"/>
+      <c r="J230" s="228"/>
+      <c r="K230" s="229"/>
       <c r="L230" s="107" t="s">
         <v>19</v>
       </c>
@@ -17364,29 +17395,29 @@
       <c r="T252" s="50"/>
     </row>
     <row r="253" spans="1:20" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A253" s="213">
+      <c r="A253" s="220">
         <v>235</v>
       </c>
-      <c r="B253" s="215">
+      <c r="B253" s="222">
         <v>45981</v>
       </c>
-      <c r="C253" s="205"/>
-      <c r="D253" s="205" t="s">
+      <c r="C253" s="212"/>
+      <c r="D253" s="212" t="s">
         <v>486</v>
       </c>
-      <c r="E253" s="205" t="s">
+      <c r="E253" s="212" t="s">
         <v>136</v>
       </c>
-      <c r="F253" s="205" t="s">
+      <c r="F253" s="212" t="s">
         <v>487</v>
       </c>
-      <c r="G253" s="205" t="s">
+      <c r="G253" s="212" t="s">
         <v>488</v>
       </c>
-      <c r="H253" s="211" t="s">
-        <v>19</v>
-      </c>
-      <c r="I253" s="211" t="s">
+      <c r="H253" s="218" t="s">
+        <v>19</v>
+      </c>
+      <c r="I253" s="218" t="s">
         <v>19</v>
       </c>
       <c r="J253" s="114" t="s">
@@ -17395,59 +17426,59 @@
       <c r="K253" s="114" t="s">
         <v>492</v>
       </c>
-      <c r="L253" s="211" t="s">
-        <v>19</v>
-      </c>
-      <c r="M253" s="205" t="s">
+      <c r="L253" s="218" t="s">
+        <v>19</v>
+      </c>
+      <c r="M253" s="212" t="s">
         <v>22</v>
       </c>
       <c r="N253" s="114" t="s">
         <v>494</v>
       </c>
-      <c r="O253" s="205" t="s">
+      <c r="O253" s="212" t="s">
         <v>496</v>
       </c>
       <c r="P253" s="114" t="s">
         <v>497</v>
       </c>
-      <c r="Q253" s="205" t="s">
-        <v>19</v>
-      </c>
-      <c r="R253" s="205" t="s">
+      <c r="Q253" s="212" t="s">
+        <v>19</v>
+      </c>
+      <c r="R253" s="212" t="s">
         <v>489</v>
       </c>
-      <c r="S253" s="193"/>
-      <c r="T253" s="179"/>
+      <c r="S253" s="210"/>
+      <c r="T253" s="186"/>
     </row>
     <row r="254" spans="1:20" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A254" s="214"/>
-      <c r="B254" s="216"/>
-      <c r="C254" s="206"/>
-      <c r="D254" s="206"/>
-      <c r="E254" s="206"/>
-      <c r="F254" s="206"/>
-      <c r="G254" s="206"/>
-      <c r="H254" s="212"/>
-      <c r="I254" s="212"/>
+      <c r="A254" s="221"/>
+      <c r="B254" s="223"/>
+      <c r="C254" s="213"/>
+      <c r="D254" s="213"/>
+      <c r="E254" s="213"/>
+      <c r="F254" s="213"/>
+      <c r="G254" s="213"/>
+      <c r="H254" s="219"/>
+      <c r="I254" s="219"/>
       <c r="J254" s="115" t="s">
         <v>491</v>
       </c>
       <c r="K254" s="115" t="s">
         <v>493</v>
       </c>
-      <c r="L254" s="212"/>
-      <c r="M254" s="206"/>
+      <c r="L254" s="219"/>
+      <c r="M254" s="213"/>
       <c r="N254" s="115" t="s">
         <v>495</v>
       </c>
-      <c r="O254" s="206"/>
+      <c r="O254" s="213"/>
       <c r="P254" s="115" t="s">
         <v>498</v>
       </c>
-      <c r="Q254" s="206"/>
-      <c r="R254" s="206"/>
-      <c r="S254" s="193"/>
-      <c r="T254" s="179"/>
+      <c r="Q254" s="213"/>
+      <c r="R254" s="213"/>
+      <c r="S254" s="210"/>
+      <c r="T254" s="186"/>
     </row>
     <row r="255" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A255" s="111">
@@ -17839,7 +17870,7 @@
       <c r="S261" s="50"/>
       <c r="T261" s="50"/>
     </row>
-    <row r="262" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A262" s="31">
         <v>243</v>
       </c>
@@ -18288,29 +18319,29 @@
       <c r="T269" s="50"/>
     </row>
     <row r="270" spans="1:20" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A270" s="207">
+      <c r="A270" s="214">
         <v>251</v>
       </c>
-      <c r="B270" s="209">
+      <c r="B270" s="216">
         <v>45982</v>
       </c>
-      <c r="C270" s="198"/>
-      <c r="D270" s="198" t="s">
+      <c r="C270" s="203"/>
+      <c r="D270" s="203" t="s">
         <v>519</v>
       </c>
-      <c r="E270" s="198" t="s">
+      <c r="E270" s="203" t="s">
         <v>321</v>
       </c>
-      <c r="F270" s="198" t="s">
+      <c r="F270" s="203" t="s">
         <v>520</v>
       </c>
-      <c r="G270" s="198" t="s">
+      <c r="G270" s="203" t="s">
         <v>18</v>
       </c>
-      <c r="H270" s="203" t="s">
-        <v>19</v>
-      </c>
-      <c r="I270" s="203" t="s">
+      <c r="H270" s="205" t="s">
+        <v>19</v>
+      </c>
+      <c r="I270" s="205" t="s">
         <v>522</v>
       </c>
       <c r="J270" s="123" t="s">
@@ -18319,8 +18350,8 @@
       <c r="K270" s="123" t="s">
         <v>525</v>
       </c>
-      <c r="L270" s="198"/>
-      <c r="M270" s="198"/>
+      <c r="L270" s="203"/>
+      <c r="M270" s="203"/>
       <c r="N270" s="123" t="s">
         <v>527</v>
       </c>
@@ -18330,33 +18361,33 @@
       <c r="P270" s="123" t="s">
         <v>531</v>
       </c>
-      <c r="Q270" s="198" t="s">
+      <c r="Q270" s="203" t="s">
         <v>533</v>
       </c>
-      <c r="R270" s="198" t="s">
+      <c r="R270" s="203" t="s">
         <v>521</v>
       </c>
-      <c r="S270" s="193"/>
-      <c r="T270" s="179"/>
+      <c r="S270" s="210"/>
+      <c r="T270" s="186"/>
     </row>
     <row r="271" spans="1:20" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A271" s="208"/>
-      <c r="B271" s="210"/>
-      <c r="C271" s="199"/>
-      <c r="D271" s="199"/>
-      <c r="E271" s="199"/>
-      <c r="F271" s="199"/>
-      <c r="G271" s="199"/>
-      <c r="H271" s="204"/>
-      <c r="I271" s="204"/>
+      <c r="A271" s="215"/>
+      <c r="B271" s="217"/>
+      <c r="C271" s="204"/>
+      <c r="D271" s="204"/>
+      <c r="E271" s="204"/>
+      <c r="F271" s="204"/>
+      <c r="G271" s="204"/>
+      <c r="H271" s="206"/>
+      <c r="I271" s="206"/>
       <c r="J271" s="124" t="s">
         <v>524</v>
       </c>
       <c r="K271" s="124" t="s">
         <v>526</v>
       </c>
-      <c r="L271" s="199"/>
-      <c r="M271" s="199"/>
+      <c r="L271" s="204"/>
+      <c r="M271" s="204"/>
       <c r="N271" s="124" t="s">
         <v>528</v>
       </c>
@@ -18366,10 +18397,10 @@
       <c r="P271" s="124" t="s">
         <v>532</v>
       </c>
-      <c r="Q271" s="199"/>
-      <c r="R271" s="199"/>
-      <c r="S271" s="193"/>
-      <c r="T271" s="179"/>
+      <c r="Q271" s="204"/>
+      <c r="R271" s="204"/>
+      <c r="S271" s="210"/>
+      <c r="T271" s="186"/>
     </row>
     <row r="272" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A272" s="120">
@@ -19041,109 +19072,109 @@
       <c r="S283" s="50"/>
       <c r="T283" s="50"/>
     </row>
-    <row r="284" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A284" s="200">
+    <row r="284" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A284" s="194">
         <v>264</v>
       </c>
-      <c r="B284" s="201">
+      <c r="B284" s="197">
         <v>45986</v>
       </c>
-      <c r="C284" s="200"/>
-      <c r="D284" s="200" t="s">
+      <c r="C284" s="194"/>
+      <c r="D284" s="194" t="s">
         <v>538</v>
       </c>
-      <c r="E284" s="200" t="s">
+      <c r="E284" s="194" t="s">
         <v>541</v>
       </c>
-      <c r="F284" s="200" t="s">
+      <c r="F284" s="194" t="s">
         <v>435</v>
       </c>
-      <c r="G284" s="202" t="s">
+      <c r="G284" s="200" t="s">
         <v>410</v>
       </c>
-      <c r="H284" s="184" t="s">
-        <v>19</v>
-      </c>
-      <c r="I284" s="190" t="s">
+      <c r="H284" s="191" t="s">
+        <v>19</v>
+      </c>
+      <c r="I284" s="208" t="s">
         <v>46</v>
       </c>
-      <c r="J284" s="184" t="s">
+      <c r="J284" s="191" t="s">
         <v>19</v>
       </c>
       <c r="K284" s="128" t="s">
         <v>542</v>
       </c>
-      <c r="L284" s="195" t="s">
-        <v>19</v>
-      </c>
-      <c r="M284" s="190" t="s">
+      <c r="L284" s="211" t="s">
+        <v>19</v>
+      </c>
+      <c r="M284" s="208" t="s">
         <v>545</v>
       </c>
-      <c r="N284" s="181" t="s">
-        <v>19</v>
-      </c>
-      <c r="O284" s="181" t="s">
-        <v>19</v>
-      </c>
-      <c r="P284" s="184" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q284" s="187">
+      <c r="N284" s="188" t="s">
+        <v>19</v>
+      </c>
+      <c r="O284" s="188" t="s">
+        <v>19</v>
+      </c>
+      <c r="P284" s="191" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q284" s="207">
         <v>46001</v>
       </c>
-      <c r="R284" s="190" t="s">
+      <c r="R284" s="208" t="s">
         <v>540</v>
       </c>
-      <c r="S284" s="193"/>
-      <c r="T284" s="179"/>
-    </row>
-    <row r="285" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A285" s="196"/>
-      <c r="B285" s="188"/>
-      <c r="C285" s="196"/>
-      <c r="D285" s="196"/>
-      <c r="E285" s="196"/>
-      <c r="F285" s="196"/>
-      <c r="G285" s="191"/>
-      <c r="H285" s="185"/>
-      <c r="I285" s="191"/>
-      <c r="J285" s="185"/>
+      <c r="S284" s="210"/>
+      <c r="T284" s="186"/>
+    </row>
+    <row r="285" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A285" s="195"/>
+      <c r="B285" s="198"/>
+      <c r="C285" s="195"/>
+      <c r="D285" s="195"/>
+      <c r="E285" s="195"/>
+      <c r="F285" s="195"/>
+      <c r="G285" s="201"/>
+      <c r="H285" s="192"/>
+      <c r="I285" s="201"/>
+      <c r="J285" s="192"/>
       <c r="K285" s="129" t="s">
         <v>543</v>
       </c>
-      <c r="L285" s="196"/>
-      <c r="M285" s="191"/>
-      <c r="N285" s="182"/>
-      <c r="O285" s="182"/>
-      <c r="P285" s="185"/>
-      <c r="Q285" s="188"/>
-      <c r="R285" s="191"/>
-      <c r="S285" s="193"/>
-      <c r="T285" s="179"/>
-    </row>
-    <row r="286" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A286" s="197"/>
-      <c r="B286" s="189"/>
-      <c r="C286" s="197"/>
-      <c r="D286" s="197"/>
-      <c r="E286" s="197"/>
-      <c r="F286" s="197"/>
-      <c r="G286" s="194"/>
-      <c r="H286" s="186"/>
-      <c r="I286" s="194"/>
-      <c r="J286" s="186"/>
+      <c r="L285" s="195"/>
+      <c r="M285" s="201"/>
+      <c r="N285" s="189"/>
+      <c r="O285" s="189"/>
+      <c r="P285" s="192"/>
+      <c r="Q285" s="198"/>
+      <c r="R285" s="201"/>
+      <c r="S285" s="210"/>
+      <c r="T285" s="186"/>
+    </row>
+    <row r="286" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A286" s="196"/>
+      <c r="B286" s="199"/>
+      <c r="C286" s="196"/>
+      <c r="D286" s="196"/>
+      <c r="E286" s="196"/>
+      <c r="F286" s="196"/>
+      <c r="G286" s="202"/>
+      <c r="H286" s="193"/>
+      <c r="I286" s="202"/>
+      <c r="J286" s="193"/>
       <c r="K286" s="130" t="s">
         <v>544</v>
       </c>
-      <c r="L286" s="197"/>
-      <c r="M286" s="194"/>
-      <c r="N286" s="183"/>
-      <c r="O286" s="183"/>
-      <c r="P286" s="186"/>
-      <c r="Q286" s="189"/>
-      <c r="R286" s="192"/>
-      <c r="S286" s="193"/>
-      <c r="T286" s="179"/>
+      <c r="L286" s="196"/>
+      <c r="M286" s="202"/>
+      <c r="N286" s="190"/>
+      <c r="O286" s="190"/>
+      <c r="P286" s="193"/>
+      <c r="Q286" s="199"/>
+      <c r="R286" s="209"/>
+      <c r="S286" s="210"/>
+      <c r="T286" s="186"/>
     </row>
     <row r="287" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A287" s="131">
@@ -21493,7 +21524,7 @@
       <c r="S328" s="50"/>
       <c r="T328" s="50"/>
     </row>
-    <row r="329" spans="1:20" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A329" s="31">
         <v>307</v>
       </c>
@@ -21549,7 +21580,7 @@
       <c r="S329" s="50"/>
       <c r="T329" s="50"/>
     </row>
-    <row r="330" spans="1:20" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A330" s="31">
         <v>308</v>
       </c>
@@ -23397,101 +23428,237 @@
       <c r="S365" s="50"/>
       <c r="T365" s="50"/>
     </row>
-    <row r="366" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A366" s="177">
-        <v>344</v>
-      </c>
-      <c r="B366" s="50"/>
-      <c r="C366" s="50"/>
-      <c r="D366" s="50"/>
-      <c r="E366" s="50"/>
-      <c r="F366" s="50"/>
-      <c r="G366" s="50"/>
-      <c r="H366" s="178"/>
-      <c r="I366" s="178"/>
-      <c r="J366" s="178"/>
-      <c r="K366" s="178"/>
-      <c r="L366" s="178"/>
-      <c r="M366" s="178"/>
-      <c r="N366" s="178"/>
-      <c r="O366" s="178"/>
-      <c r="P366" s="178"/>
-      <c r="Q366" s="178"/>
-      <c r="R366" s="178"/>
-      <c r="S366" s="50"/>
-      <c r="T366" s="50"/>
-    </row>
-    <row r="367" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A367" s="177">
-        <v>345</v>
-      </c>
-      <c r="B367" s="178"/>
-      <c r="C367" s="178"/>
-      <c r="D367" s="178"/>
-      <c r="E367" s="178"/>
-      <c r="F367" s="178"/>
-      <c r="G367" s="178"/>
-      <c r="H367" s="178"/>
-      <c r="I367" s="178"/>
-      <c r="J367" s="178"/>
-      <c r="K367" s="178"/>
-      <c r="L367" s="178"/>
-      <c r="M367" s="178"/>
-      <c r="N367" s="178"/>
-      <c r="O367" s="178"/>
-      <c r="P367" s="178"/>
-      <c r="Q367" s="178"/>
-      <c r="R367" s="178"/>
-      <c r="S367" s="50"/>
-      <c r="T367" s="50"/>
-    </row>
-    <row r="368" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A368" s="177">
-        <v>346</v>
-      </c>
-      <c r="B368" s="178"/>
-      <c r="C368" s="178"/>
-      <c r="D368" s="178"/>
-      <c r="E368" s="178"/>
-      <c r="F368" s="178"/>
-      <c r="G368" s="178"/>
-      <c r="H368" s="178"/>
-      <c r="I368" s="178"/>
-      <c r="J368" s="178"/>
-      <c r="K368" s="178"/>
-      <c r="L368" s="178"/>
-      <c r="M368" s="178"/>
-      <c r="N368" s="178"/>
-      <c r="O368" s="178"/>
-      <c r="P368" s="178"/>
-      <c r="Q368" s="178"/>
-      <c r="R368" s="178"/>
-      <c r="S368" s="50"/>
-      <c r="T368" s="50"/>
-    </row>
-    <row r="369" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A369" s="177">
-        <v>347</v>
-      </c>
-      <c r="B369" s="178"/>
-      <c r="C369" s="178"/>
-      <c r="D369" s="178"/>
-      <c r="E369" s="178"/>
-      <c r="F369" s="178"/>
-      <c r="G369" s="178"/>
-      <c r="H369" s="178"/>
-      <c r="I369" s="178"/>
-      <c r="J369" s="178"/>
-      <c r="K369" s="178"/>
-      <c r="L369" s="178"/>
-      <c r="M369" s="178"/>
-      <c r="N369" s="178"/>
-      <c r="O369" s="178"/>
-      <c r="P369" s="178"/>
-      <c r="Q369" s="178"/>
-      <c r="R369" s="178"/>
-      <c r="S369" s="50"/>
-      <c r="T369" s="50"/>
+    <row r="366" spans="1:20" s="185" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A366" s="179">
+        <v>343</v>
+      </c>
+      <c r="B366" s="180">
+        <v>45992</v>
+      </c>
+      <c r="C366" s="181" t="s">
+        <v>14</v>
+      </c>
+      <c r="D366" s="181" t="s">
+        <v>15</v>
+      </c>
+      <c r="E366" s="181" t="s">
+        <v>16</v>
+      </c>
+      <c r="F366" s="181" t="s">
+        <v>17</v>
+      </c>
+      <c r="G366" s="181" t="s">
+        <v>657</v>
+      </c>
+      <c r="H366" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="I366" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="J366" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="K366" s="181" t="s">
+        <v>20</v>
+      </c>
+      <c r="L366" s="181" t="s">
+        <v>21</v>
+      </c>
+      <c r="M366" s="181" t="s">
+        <v>22</v>
+      </c>
+      <c r="N366" s="181">
+        <v>21</v>
+      </c>
+      <c r="O366" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="P366" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q366" s="180">
+        <v>46032</v>
+      </c>
+      <c r="R366" s="182" t="s">
+        <v>23</v>
+      </c>
+      <c r="S366" s="183"/>
+      <c r="T366" s="184"/>
+    </row>
+    <row r="367" spans="1:20" s="185" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A367" s="179">
+        <v>343</v>
+      </c>
+      <c r="B367" s="180">
+        <v>45993</v>
+      </c>
+      <c r="C367" s="181" t="s">
+        <v>14</v>
+      </c>
+      <c r="D367" s="181" t="s">
+        <v>15</v>
+      </c>
+      <c r="E367" s="181" t="s">
+        <v>24</v>
+      </c>
+      <c r="F367" s="181" t="s">
+        <v>17</v>
+      </c>
+      <c r="G367" s="181" t="s">
+        <v>657</v>
+      </c>
+      <c r="H367" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="I367" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="J367" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="K367" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="L367" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="M367" s="181" t="s">
+        <v>22</v>
+      </c>
+      <c r="N367" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="O367" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="P367" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q367" s="180">
+        <v>46033</v>
+      </c>
+      <c r="R367" s="182" t="s">
+        <v>23</v>
+      </c>
+      <c r="S367" s="183"/>
+      <c r="T367" s="184"/>
+    </row>
+    <row r="368" spans="1:20" s="185" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A368" s="179">
+        <v>343</v>
+      </c>
+      <c r="B368" s="180">
+        <v>45994</v>
+      </c>
+      <c r="C368" s="181" t="s">
+        <v>14</v>
+      </c>
+      <c r="D368" s="181" t="s">
+        <v>15</v>
+      </c>
+      <c r="E368" s="181" t="s">
+        <v>25</v>
+      </c>
+      <c r="F368" s="181" t="s">
+        <v>17</v>
+      </c>
+      <c r="G368" s="181" t="s">
+        <v>657</v>
+      </c>
+      <c r="H368" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="I368" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="J368" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="K368" s="181" t="s">
+        <v>26</v>
+      </c>
+      <c r="L368" s="181" t="s">
+        <v>21</v>
+      </c>
+      <c r="M368" s="181" t="s">
+        <v>22</v>
+      </c>
+      <c r="N368" s="181">
+        <v>21</v>
+      </c>
+      <c r="O368" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="P368" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q368" s="180">
+        <v>46034</v>
+      </c>
+      <c r="R368" s="182" t="s">
+        <v>23</v>
+      </c>
+      <c r="S368" s="183"/>
+      <c r="T368" s="184"/>
+    </row>
+    <row r="369" spans="1:20" s="185" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A369" s="179">
+        <v>343</v>
+      </c>
+      <c r="B369" s="180">
+        <v>45995</v>
+      </c>
+      <c r="C369" s="181" t="s">
+        <v>14</v>
+      </c>
+      <c r="D369" s="181" t="s">
+        <v>15</v>
+      </c>
+      <c r="E369" s="181" t="s">
+        <v>27</v>
+      </c>
+      <c r="F369" s="181" t="s">
+        <v>17</v>
+      </c>
+      <c r="G369" s="181" t="s">
+        <v>657</v>
+      </c>
+      <c r="H369" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="I369" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="J369" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="K369" s="181" t="s">
+        <v>28</v>
+      </c>
+      <c r="L369" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="M369" s="181" t="s">
+        <v>22</v>
+      </c>
+      <c r="N369" s="181">
+        <v>21</v>
+      </c>
+      <c r="O369" s="181" t="s">
+        <v>29</v>
+      </c>
+      <c r="P369" s="181" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q369" s="180">
+        <v>46035</v>
+      </c>
+      <c r="R369" s="182" t="s">
+        <v>23</v>
+      </c>
+      <c r="S369" s="183"/>
+      <c r="T369" s="184"/>
     </row>
     <row r="370" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A370" s="177">
@@ -25342,8 +25509,8 @@
       <c r="T446" s="50"/>
     </row>
     <row r="447" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A447" s="180"/>
-      <c r="B447" s="180"/>
+      <c r="A447" s="187"/>
+      <c r="B447" s="187"/>
       <c r="C447" s="50"/>
       <c r="D447" s="50"/>
       <c r="E447" s="50"/>
@@ -25364,8 +25531,8 @@
       <c r="T447" s="50"/>
     </row>
     <row r="448" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A448" s="179"/>
-      <c r="B448" s="179"/>
+      <c r="A448" s="186"/>
+      <c r="B448" s="186"/>
       <c r="C448" s="50"/>
       <c r="D448" s="50"/>
       <c r="E448" s="50"/>
@@ -25386,8 +25553,8 @@
       <c r="T448" s="50"/>
     </row>
     <row r="449" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A449" s="179"/>
-      <c r="B449" s="179"/>
+      <c r="A449" s="186"/>
+      <c r="B449" s="186"/>
       <c r="C449" s="50"/>
       <c r="D449" s="50"/>
       <c r="E449" s="50"/>
@@ -25408,8 +25575,8 @@
       <c r="T449" s="50"/>
     </row>
     <row r="450" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A450" s="179"/>
-      <c r="B450" s="179"/>
+      <c r="A450" s="186"/>
+      <c r="B450" s="186"/>
       <c r="C450" s="50"/>
       <c r="D450" s="50"/>
       <c r="E450" s="50"/>
@@ -25430,8 +25597,8 @@
       <c r="T450" s="50"/>
     </row>
     <row r="451" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A451" s="179"/>
-      <c r="B451" s="179"/>
+      <c r="A451" s="186"/>
+      <c r="B451" s="186"/>
       <c r="C451" s="50"/>
       <c r="D451" s="50"/>
       <c r="E451" s="50"/>
@@ -25452,8 +25619,8 @@
       <c r="T451" s="50"/>
     </row>
     <row r="452" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A452" s="179"/>
-      <c r="B452" s="179"/>
+      <c r="A452" s="186"/>
+      <c r="B452" s="186"/>
       <c r="C452" s="50"/>
       <c r="D452" s="50"/>
       <c r="E452" s="50"/>
@@ -25474,8 +25641,8 @@
       <c r="T452" s="50"/>
     </row>
     <row r="453" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A453" s="179"/>
-      <c r="B453" s="179"/>
+      <c r="A453" s="186"/>
+      <c r="B453" s="186"/>
       <c r="C453" s="50"/>
       <c r="D453" s="50"/>
       <c r="E453" s="50"/>
@@ -25497,8 +25664,6 @@
     </row>
   </sheetData>
   <mergeCells count="301">
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="E25:E26"/>
@@ -25525,6 +25690,11 @@
     <mergeCell ref="R30:R31"/>
     <mergeCell ref="S30:S31"/>
     <mergeCell ref="T30:T31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="O30:O31"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="C32:C33"/>
@@ -25534,9 +25704,6 @@
     <mergeCell ref="G30:G31"/>
     <mergeCell ref="J30:J31"/>
     <mergeCell ref="K30:K31"/>
-    <mergeCell ref="L30:L31"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="O30:O31"/>
     <mergeCell ref="O32:O33"/>
     <mergeCell ref="Q32:Q33"/>
     <mergeCell ref="R32:R33"/>

</xml_diff>